<commit_message>
Finally got Nashville sorted
</commit_message>
<xml_diff>
--- a/data/input_data_US_nash.xlsx
+++ b/data/input_data_US_nash.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominic.delport\Documents\GitHub\covasim-australia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B84DF5-44DE-4D09-8160-CDE2DE7FF3C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4EA006-95C7-40BC-9C81-52A8F0D5F83A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="839" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="839" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="age_sex" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="102">
   <si>
     <t>0-4</t>
   </si>
@@ -380,6 +380,18 @@
   </si>
   <si>
     <t>Retail, commerical, entertainment open to 75%, restaurants to 50%, gatherings limited to 25</t>
+  </si>
+  <si>
+    <t>lockdown5</t>
+  </si>
+  <si>
+    <t>Hypothetical restrictions</t>
+  </si>
+  <si>
+    <t>lockdown6</t>
+  </si>
+  <si>
+    <t>Hypothetical restrictions (relaxed)</t>
   </si>
 </sst>
 </file>
@@ -724,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -836,9 +848,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5155,10 +5164,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5258,7 +5267,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="62"/>
+      <c r="A3" s="61"/>
       <c r="B3" s="35" t="s">
         <v>69</v>
       </c>
@@ -5289,12 +5298,12 @@
         <v>43911</v>
       </c>
       <c r="M3" s="54">
-        <f t="shared" ref="M3:M7" si="0">L4</f>
+        <f t="shared" ref="M3:M6" si="0">L4</f>
         <v>43913</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="62"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="35" t="s">
         <v>70</v>
       </c>
@@ -5330,7 +5339,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="62"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="35" t="s">
         <v>71</v>
       </c>
@@ -5366,7 +5375,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="62"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="35" t="s">
         <v>72</v>
       </c>
@@ -5402,7 +5411,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="62"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="35" t="s">
         <v>73</v>
       </c>
@@ -5433,46 +5442,108 @@
         <v>44004</v>
       </c>
       <c r="M7" s="54">
-        <f t="shared" si="0"/>
+        <f>L8</f>
         <v>44015</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="63"/>
-      <c r="B8" s="27" t="s">
+      <c r="A8" s="61"/>
+      <c r="B8" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="38">
         <v>0.65</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="36">
         <v>1</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="36">
         <v>1</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="36">
         <v>1</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="36">
         <v>1</v>
       </c>
-      <c r="I8" s="21">
-        <v>0</v>
-      </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="57">
+      <c r="I8" s="36">
+        <v>0</v>
+      </c>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="56">
         <v>44015</v>
       </c>
-      <c r="M8" s="55"/>
+      <c r="M8" s="54"/>
+    </row>
+    <row r="9" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="61"/>
+      <c r="B9" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="38">
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="36">
+        <v>1</v>
+      </c>
+      <c r="F9" s="36">
+        <v>1</v>
+      </c>
+      <c r="G9" s="36">
+        <v>1</v>
+      </c>
+      <c r="H9" s="36">
+        <v>1</v>
+      </c>
+      <c r="I9" s="36">
+        <v>0</v>
+      </c>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="54"/>
+    </row>
+    <row r="10" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="62"/>
+      <c r="B10" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="40">
+        <v>0.65</v>
+      </c>
+      <c r="E10" s="21">
+        <v>1</v>
+      </c>
+      <c r="F10" s="21">
+        <v>1</v>
+      </c>
+      <c r="G10" s="21">
+        <v>1</v>
+      </c>
+      <c r="H10" s="21">
+        <v>1</v>
+      </c>
+      <c r="I10" s="21">
+        <v>0</v>
+      </c>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A2:A10"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update brazil and nashville
</commit_message>
<xml_diff>
--- a/data/input_data_US_nash.xlsx
+++ b/data/input_data_US_nash.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominic.delport\Documents\GitHub\covasim-australia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4EA006-95C7-40BC-9C81-52A8F0D5F83A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AD0F7D-023C-4291-9F31-7EE71C691EBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="839" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5167,7 +5167,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>